<commit_message>
Add progress report and update risk management
</commit_message>
<xml_diff>
--- a/docs/iter0/CS673_SPPP_RiskManagement_team1.xlsx
+++ b/docs/iter0/CS673_SPPP_RiskManagement_team1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faubertdor/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faubertdor/Documents/MS Software Development/MET CS 673/Term Project/Iter0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74F0C19-DB7B-0548-88A0-7D81FEB89EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1FE19F-CBF7-8F4B-8A66-BDC1A5408EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -764,12 +764,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="65" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" style="2" customWidth="1"/>
@@ -821,7 +821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="97" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -875,7 +875,7 @@
       <c r="Z2" s="8"/>
       <c r="AA2" s="8"/>
     </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>19</v>
@@ -927,7 +927,7 @@
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
     </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>23</v>
@@ -979,7 +979,7 @@
       <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
     </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1033,7 +1033,7 @@
       <c r="Z5" s="8"/>
       <c r="AA5" s="8"/>
     </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>33</v>
@@ -1085,7 +1085,7 @@
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
     </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="Z7" s="8"/>
       <c r="AA7" s="8"/>
     </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>42</v>
@@ -1243,7 +1243,7 @@
       <c r="Z9" s="8"/>
       <c r="AA9" s="8"/>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="76" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>49</v>
       </c>
@@ -1349,7 +1349,7 @@
       <c r="Z11" s="8"/>
       <c r="AA11" s="8"/>
     </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>57</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="Z13" s="8"/>
       <c r="AA13" s="8"/>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>67</v>
       </c>
@@ -1509,7 +1509,7 @@
       <c r="Z14" s="8"/>
       <c r="AA14" s="8"/>
     </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>71</v>
       </c>
@@ -1563,7 +1563,7 @@
       <c r="Z15" s="8"/>
       <c r="AA15" s="8"/>
     </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="101" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>75</v>
       </c>

</xml_diff>